<commit_message>
modified the specs and design based on new ideas and conversations.
</commit_message>
<xml_diff>
--- a/electronics/hoektronics-cnc-controller/pin-allocation.xlsx
+++ b/electronics/hoektronics-cnc-controller/pin-allocation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="136">
   <si>
     <t>Pin Name</t>
   </si>
@@ -94,21 +94,12 @@
     <t>buzzer</t>
   </si>
   <si>
-    <t>pwm mosfets</t>
-  </si>
-  <si>
-    <t>analog inputs</t>
-  </si>
-  <si>
     <t>current monitoring</t>
   </si>
   <si>
     <t>spindle rpm</t>
   </si>
   <si>
-    <t>axes encoders</t>
-  </si>
-  <si>
     <t>axes endstops</t>
   </si>
   <si>
@@ -316,36 +307,6 @@
     <t>P1.18</t>
   </si>
   <si>
-    <t>XQUADA</t>
-  </si>
-  <si>
-    <t>XQUADB</t>
-  </si>
-  <si>
-    <t>YQUADA</t>
-  </si>
-  <si>
-    <t>YQUADB</t>
-  </si>
-  <si>
-    <t>ZQUADA</t>
-  </si>
-  <si>
-    <t>ZQUADB</t>
-  </si>
-  <si>
-    <t>AQUADA</t>
-  </si>
-  <si>
-    <t>AQUADB</t>
-  </si>
-  <si>
-    <t>BQUADA</t>
-  </si>
-  <si>
-    <t>BQUADB</t>
-  </si>
-  <si>
     <t>XSTOP</t>
   </si>
   <si>
@@ -358,9 +319,6 @@
     <t>ASTOP</t>
   </si>
   <si>
-    <t>BSTOP</t>
-  </si>
-  <si>
     <t>DOOR</t>
   </si>
   <si>
@@ -373,15 +331,6 @@
     <t>MOSFET</t>
   </si>
   <si>
-    <t>BSTEP</t>
-  </si>
-  <si>
-    <t>BENABLE</t>
-  </si>
-  <si>
-    <t>BDIR</t>
-  </si>
-  <si>
     <t>ASTEP</t>
   </si>
   <si>
@@ -433,18 +382,9 @@
     <t>CURRENT-</t>
   </si>
   <si>
-    <t>ADC1</t>
-  </si>
-  <si>
-    <t>ADC2</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
-    <t>more todo:</t>
-  </si>
-  <si>
     <t>test all footprints</t>
   </si>
   <si>
@@ -460,9 +400,6 @@
     <t>a protect</t>
   </si>
   <si>
-    <t>b protect</t>
-  </si>
-  <si>
     <t>BUZZER</t>
   </si>
   <si>
@@ -470,6 +407,27 @@
   </si>
   <si>
     <t>VOUT</t>
+  </si>
+  <si>
+    <t>create eagle module for RN-131</t>
+  </si>
+  <si>
+    <t>wire up the RN-42 bluetooth module</t>
+  </si>
+  <si>
+    <t>wire up the RN-131 module</t>
+  </si>
+  <si>
+    <t>re-verify all the pin assignments</t>
+  </si>
+  <si>
+    <t>re-layout the board</t>
+  </si>
+  <si>
+    <t>todo:</t>
+  </si>
+  <si>
+    <t>vacuum on/off</t>
   </si>
 </sst>
 </file>
@@ -560,8 +518,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -684,7 +646,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -736,6 +698,8 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -787,6 +751,8 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1116,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1148,68 +1114,67 @@
         <v>15</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D4" si="0">B3*C3</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
         <f>C3</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="2">
-        <v>2</v>
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5">
-        <f>C3</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ref="D5:D15" si="1">B5*C5</f>
-        <v>10</v>
+        <f t="shared" ref="D5:D13" si="1">B5*C5</f>
+        <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1222,53 +1187,53 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" s="2">
@@ -1276,12 +1241,12 @@
         <v>1</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1293,9 +1258,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>123</v>
-      </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
@@ -1312,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1330,7 +1293,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1338,95 +1301,84 @@
         <v>24</v>
       </c>
       <c r="B13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
-        <v>3</v>
-      </c>
-      <c r="D14" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>123</v>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3">
+        <f>SUM(D3:D13)</f>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>123</v>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="3">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3">
-        <f>SUM(D3:D15)</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="3">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="3">
-        <f>D17-D16</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <f>D15-D14</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1444,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1455,17 +1407,17 @@
   <sheetData>
     <row r="1" spans="1:11" ht="20">
       <c r="A1" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="I1" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
@@ -1478,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
@@ -1487,7 +1439,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>0</v>
@@ -1496,12 +1448,12 @@
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1510,27 +1462,25 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>118</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="G3" s="4"/>
       <c r="I3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J3" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1539,24 +1489,24 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="I4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1565,151 +1515,147 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="I6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="C7" s="4"/>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>119</v>
-      </c>
+      <c r="C8" s="4"/>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="I10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -1718,24 +1664,24 @@
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="I11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -1744,223 +1690,195 @@
         <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="I12" t="s">
-        <v>88</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>98</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="G13" s="4"/>
       <c r="I13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G14" s="4"/>
       <c r="I14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="C15" s="4"/>
       <c r="E15" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>100</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="G15" s="4"/>
       <c r="I15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>101</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="G16" s="4"/>
       <c r="I16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="C17" s="4"/>
       <c r="E17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>102</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G17" s="4"/>
       <c r="I17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>103</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="G18" s="4"/>
       <c r="I18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="I19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>112</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C21" s="4"/>
       <c r="I21" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>104</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>105</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>106</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>107</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>